<commit_message>
Mise à jour de fichier1 et fichier2
</commit_message>
<xml_diff>
--- a/cotisations.xlsx
+++ b/cotisations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\cotisation_streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE392B6-9F91-4837-987C-0A7EB37E7411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DEBC1F-1522-4CB2-80A6-C9D66DC2B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D47798F2-2E3F-4123-AE53-AE0EE02E72EF}"/>
   </bookViews>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FEF14F-85DA-4ECB-B2FA-74F479AC4B4A}">
   <dimension ref="A1:D290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="G196" sqref="G196"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Mise à jour du fichier cotisations.xlsx
</commit_message>
<xml_diff>
--- a/cotisations.xlsx
+++ b/cotisations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\cotisation_streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DEBC1F-1522-4CB2-80A6-C9D66DC2B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6002160-93CE-4F14-A4AA-2D08940BF0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D47798F2-2E3F-4123-AE53-AE0EE02E72EF}"/>
   </bookViews>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FEF14F-85DA-4ECB-B2FA-74F479AC4B4A}">
   <dimension ref="A1:D290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="G279" sqref="G279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3447,7 +3447,7 @@
         <v>9</v>
       </c>
       <c r="D210" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
@@ -3461,7 +3461,7 @@
         <v>10</v>
       </c>
       <c r="D211" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
@@ -3475,7 +3475,7 @@
         <v>11</v>
       </c>
       <c r="D212" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
@@ -3489,7 +3489,7 @@
         <v>12</v>
       </c>
       <c r="D213" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
@@ -3503,7 +3503,7 @@
         <v>13</v>
       </c>
       <c r="D214" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
@@ -3517,7 +3517,7 @@
         <v>14</v>
       </c>
       <c r="D215" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
@@ -3531,7 +3531,7 @@
         <v>15</v>
       </c>
       <c r="D216" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
@@ -3545,7 +3545,7 @@
         <v>16</v>
       </c>
       <c r="D217" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
@@ -4399,7 +4399,7 @@
         <v>5</v>
       </c>
       <c r="D278" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.35">
@@ -4413,7 +4413,7 @@
         <v>6</v>
       </c>
       <c r="D279" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>